<commit_message>
LM393 code and other data upladed
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t xml:space="preserve">Progress Report</t>
   </si>
@@ -76,31 +76,63 @@
     <t xml:space="preserve">Search Component to preferd for our stm32 board and  contact with component dealer.</t>
   </si>
   <si>
-    <t xml:space="preserve">can </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.CAN protocol reference model layers          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. CAN bus , recessive bits , dominant bus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.CAN frame structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. CAN network topology</t>
+    <t xml:space="preserve">.........</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 ...........</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              ...........</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            ...........</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             ...........</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CAN protocol reference model layers ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CAN bus , recessive bits , dominant bus</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN frame structure and CAN network topology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the datasheet of LM393 Rain water sensor &amp; pin configuration is done with STM board.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the obtainable value of LM393 with ADC .See the ADC and UART code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done the coding of LM393 Rain Water Sesor using ADC and UART And upload on Git.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -142,6 +174,20 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,8 +310,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -345,10 +395,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,46 +619,60 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
-        <v>45252</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <v>45253</v>
-      </c>
-      <c r="B20" s="7"/>
+        <v>45285</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <v>45254</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+        <v>45286</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <v>45255</v>
+        <v>45287</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <v>45256</v>
+        <v>45288</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -617,16 +681,18 @@
     </row>
     <row r="24" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <v>45257</v>
+        <v>45289</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
-        <v>45258</v>
+        <v>45290</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -635,7 +701,7 @@
     </row>
     <row r="26" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <v>45259</v>
+        <v>45291</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -644,7 +710,7 @@
     </row>
     <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <v>45260</v>
+        <v>45292</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -653,7 +719,7 @@
     </row>
     <row r="28" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
-        <v>45261</v>
+        <v>45293</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -662,7 +728,7 @@
     </row>
     <row r="29" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
-        <v>45262</v>
+        <v>45294</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -671,7 +737,7 @@
     </row>
     <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
-        <v>45263</v>
+        <v>45295</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -680,7 +746,7 @@
     </row>
     <row r="31" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
-        <v>45264</v>
+        <v>45296</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -689,7 +755,7 @@
     </row>
     <row r="32" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
-        <v>45265</v>
+        <v>45297</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -698,38 +764,15 @@
     </row>
     <row r="33" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
-        <v>45266</v>
+        <v>45298</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="n">
-        <v>45285</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0" t="s">
-        <v>22</v>
-      </c>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated in progress report
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t xml:space="preserve">Progress Report</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reading about temperature sensor LM35 and DS18B20 Water proof tempearature sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC and UART sensor code done</t>
   </si>
 </sst>
 </file>
@@ -120,7 +123,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,12 +169,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -261,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,11 +295,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,8 +378,8 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -722,7 +715,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="7"/>
@@ -751,11 +744,13 @@
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
+      <c r="A34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
CAN BASIC CODE and can filters
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t xml:space="preserve">Progress Report</t>
   </si>
@@ -115,7 +115,13 @@
     <t xml:space="preserve">ADC and UART sensor code done</t>
   </si>
   <si>
+    <t xml:space="preserve">reading about can filter and logical characteristics</t>
+  </si>
+  <si>
     <t xml:space="preserve">Merge the sensor code in Final_sens_intr directory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Project Evaluation-2 and basic code of CAN communication is done with LED </t>
   </si>
   <si>
     <t xml:space="preserve">Project Evolution -2</t>
@@ -129,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -175,12 +181,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -268,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,15 +305,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,8 +392,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,28 +794,30 @@
       <c r="A36" s="5" t="n">
         <v>45302</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="9" t="s">
+      <c r="B36" s="7" t="s">
         <v>31</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="9" t="n">
         <v>45303</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>32</v>
+      <c r="B37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>